<commit_message>
Add missing curation statuses
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Environmental_system_Defs.xlsx
+++ b/inputs/AddictO_Environmental_system_Defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FDBE2-C358-0A43-AC58-07BA80106052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F597C8FC-2E38-F044-BDC1-0E40EEFEECAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="163">
   <si>
     <t>ID</t>
   </si>
@@ -1039,8 +1039,8 @@
   <dimension ref="A1:R2813"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I77" sqref="I77"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1967,6 +1967,9 @@
       <c r="G30" s="11" t="s">
         <v>88</v>
       </c>
+      <c r="Q30" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="R30" s="9"/>
     </row>
     <row r="31" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2077,6 +2080,9 @@
       <c r="H34" s="15"/>
       <c r="I34" s="4" t="s">
         <v>158</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="R34" s="9"/>
     </row>

</xml_diff>

<commit_message>
Adding Reviewer query column
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Environmental_system_Defs.xlsx
+++ b/inputs/AddictO_Environmental_system_Defs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F597C8FC-2E38-F044-BDC1-0E40EEFEECAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2284CB32-E469-5E4D-80BC-3FA8608B80C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>state</t>
+  </si>
+  <si>
+    <t>Reviewer query</t>
   </si>
 </sst>
 </file>
@@ -1036,11 +1039,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2813"/>
+  <dimension ref="A1:S2813"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q35" sqref="Q35"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1063,11 +1066,12 @@
     <col min="16" max="16" width="9.1640625" style="4" customWidth="1"/>
     <col min="17" max="17" width="13.5" style="4" customWidth="1"/>
     <col min="18" max="18" width="24.6640625" style="4" customWidth="1"/>
-    <col min="19" max="22" width="9.1640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" style="4" customWidth="1"/>
+    <col min="20" max="22" width="9.1640625" style="4" customWidth="1"/>
     <col min="23" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1122,8 +1126,11 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>18</v>
       </c>
@@ -1159,7 +1166,7 @@
       </c>
       <c r="R2" s="32"/>
     </row>
-    <row r="3" spans="1:18" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1195,7 +1202,7 @@
       </c>
       <c r="R3" s="9"/>
     </row>
-    <row r="4" spans="1:18" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1231,7 +1238,7 @@
       </c>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -1265,7 +1272,7 @@
       </c>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>40</v>
       </c>
@@ -1299,7 +1306,7 @@
       </c>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="18" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -1333,7 +1340,7 @@
       </c>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>48</v>
       </c>
@@ -1366,7 +1373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>52</v>
       </c>
@@ -1399,7 +1406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>61</v>
@@ -1463,7 +1470,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="9" t="s">
         <v>150</v>
@@ -1489,7 +1496,7 @@
       </c>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>62</v>
       </c>
@@ -1525,7 +1532,7 @@
       </c>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>67</v>
@@ -1551,7 +1558,7 @@
       </c>
       <c r="R14" s="5"/>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>68</v>
@@ -1577,7 +1584,7 @@
       </c>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="9" t="s">
         <v>69</v>

</xml_diff>